<commit_message>
Kingdom api 작성중 (MapSnapshot json 저장방식으로 변경)
</commit_message>
<xml_diff>
--- a/Data/Excel/Model/User/Player.xlsx
+++ b/Data/Excel/Model/User/Player.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Model\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482DD0B6-9886-42BB-AC15-3F5476BDF952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1634D7A-D7C5-486B-BBF6-52EF86A8092D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Packet" sheetId="1" r:id="rId1"/>
@@ -205,23 +205,23 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>CastleLv</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemList</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIST:ItemPacket</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>PlacedKingdomItemList</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>LIST:PlacedKingdomItemPacket</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CastleLv</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemList</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIST:ItemPacket</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1158,19 +1158,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1245,9 +1245,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -1256,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1441,18 +1441,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1474,12 +1474,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E30" t="s">
         <v>33</v>

</xml_diff>